<commit_message>
finish responsive home page
</commit_message>
<xml_diff>
--- a/Usecase.xlsx
+++ b/Usecase.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Front\Flash Card\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Front\FlashCard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27515D07-52E4-4458-9A14-7BE47686A29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62518E74-ADEA-4848-8C86-B96E4C435636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NextJS" sheetId="3" r:id="rId1"/>
+    <sheet name="Database" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="102">
   <si>
     <t>Home</t>
   </si>
@@ -201,12 +202,6 @@
     <t>Current learn time</t>
   </si>
   <si>
-    <t>Space will flip/card the card.  Next will call next card. Pre will reflip the card</t>
-  </si>
-  <si>
-    <t>Linear learning</t>
-  </si>
-  <si>
     <t>Ending</t>
   </si>
   <si>
@@ -285,17 +280,65 @@
     <t>Export / Share / Clone / Delete</t>
   </si>
   <si>
-    <t>Create → course detail</t>
-  </si>
-  <si>
     <t>(both 2 model dialog)</t>
+  </si>
+  <si>
+    <t>Pack</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>learnedTimes</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>starFocus</t>
+  </si>
+  <si>
+    <t>wrongCount</t>
+  </si>
+  <si>
+    <t>bestTime</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>bestRecord</t>
+  </si>
+  <si>
+    <t>lastLearn</t>
+  </si>
+  <si>
+    <t>learningSet</t>
+  </si>
+  <si>
+    <t>Space will flip/next the card.  Next will call next card. Pre will reflip the card</t>
+  </si>
+  <si>
+    <t>OnlySpace</t>
+  </si>
+  <si>
+    <t>Packs</t>
+  </si>
+  <si>
+    <t>id[]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +356,22 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Bellota"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -350,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,6 +432,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63354B96-9DFA-4E4C-B699-5D5857C739DB}">
   <dimension ref="A1:AO36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.45"/>
@@ -700,7 +761,7 @@
         <v>10</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.45">
@@ -712,16 +773,16 @@
         <v>32</v>
       </c>
       <c r="S2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.45">
@@ -738,16 +799,16 @@
         <v>33</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.45">
@@ -755,10 +816,10 @@
         <v>5</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.45">
@@ -769,10 +830,10 @@
         <v>42</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.45">
@@ -794,19 +855,19 @@
         <v>3</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.45">
@@ -826,15 +887,15 @@
         <v>54</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="C9" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>38</v>
@@ -849,7 +910,7 @@
         <v>53</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.45">
@@ -863,7 +924,7 @@
         <v>43</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.45">
@@ -876,7 +937,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>41</v>
@@ -900,10 +961,10 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.45">
       <c r="K15" s="9" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="P15" s="2"/>
     </row>
@@ -1013,35 +1074,128 @@
     </row>
     <row r="30" spans="10:13" x14ac:dyDescent="0.45">
       <c r="J30" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="10:13" x14ac:dyDescent="0.45">
       <c r="K31" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="10:13" x14ac:dyDescent="0.45">
       <c r="K32" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K33" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K34" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K36" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01ED0B9-3027-4E1B-825A-77729C556B9C}">
+  <dimension ref="B2:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>